<commit_message>
drew the categorized benchmark charts
</commit_message>
<xml_diff>
--- a/data/GitAndroidAnalysis/accuracy_analysis2/curve_for_weight_adjustment.xlsx
+++ b/data/GitAndroidAnalysis/accuracy_analysis2/curve_for_weight_adjustment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\DESKTOP-NTK8GIP\d\ResearchSpace\ResearchProjects\UMLx\data\GitAndroidAnalysis\accuracy_analysis2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ResearchSpace\ResearchProjects\UMLx\data\GitAndroidAnalysis\accuracy_analysis2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90BB3465-A8E8-41AA-900F-C46D7396B861}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EB20746-3129-4B9A-B1A8-F4F7C750B79A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9525" xr2:uid="{985EAFBB-D308-49E7-BBB0-9AE92E659F37}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="21954" windowHeight="11860" xr2:uid="{985EAFBB-D308-49E7-BBB0-9AE92E659F37}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,12 +30,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Bayes</t>
+    <t>Prior</t>
   </si>
   <si>
-    <t>Prior</t>
+    <t>SWTIII</t>
+  </si>
+  <si>
+    <t>SWTII</t>
   </si>
 </sst>
 </file>
@@ -119,13 +122,13 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Bayes</c:v>
+                  <c:v>SWTIII</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -134,8 +137,8 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="diamond"/>
-            <c:size val="6"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
@@ -144,12 +147,179 @@
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
-                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.0088203042550852E-2"/>
+                  <c:y val="-6.7224755648599794E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000014-1CEA-4585-BB20-DDC841D239A5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.1414861300084502E-2"/>
+                  <c:y val="-3.3612510156496057E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:noAutofit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="75000"/>
+                          <a:lumOff val="25000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="2.8357320254781063E-2"/>
+                      <c:h val="5.0368280501909543E-2"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000013-1CEA-4585-BB20-DDC841D239A5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.5604603028274477E-3"/>
+                  <c:y val="-1.3444951129719959E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000012-1CEA-4585-BB20-DDC841D239A5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.1414861300084535E-2"/>
+                  <c:y val="-3.6973615606729883E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000011-1CEA-4585-BB20-DDC841D239A5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.6668648529286735E-2"/>
+                  <c:y val="-2.6889902259439918E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000C-1CEA-4585-BB20-DDC841D239A5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.6131868437981773E-2"/>
+                  <c:y val="-2.3528664477009988E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-1CEA-4585-BB20-DDC841D239A5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -167,8 +337,8 @@
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
-                        <a:lumMod val="50000"/>
-                        <a:lumOff val="50000"/>
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -192,13 +362,14 @@
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
-                    <a:ln w="9525">
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                       <a:solidFill>
                         <a:schemeClr val="tx1">
                           <a:lumMod val="35000"/>
                           <a:lumOff val="65000"/>
                         </a:schemeClr>
                       </a:solidFill>
+                      <a:round/>
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
@@ -239,7 +410,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5A49-414F-BAAD-551BD7DC5A21}"/>
+              <c16:uniqueId val="{00000000-1CEA-4585-BB20-DDC841D239A5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -252,13 +423,13 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Prior</c:v>
+                  <c:v>SWTII</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -267,8 +438,8 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="6"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
@@ -277,12 +448,121 @@
                 <a:solidFill>
                   <a:schemeClr val="accent2"/>
                 </a:solidFill>
-                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.7458526695515425E-2"/>
+                  <c:y val="2.3528664477009926E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000010-1CEA-4585-BB20-DDC841D239A5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.008820304255092E-2"/>
+                  <c:y val="2.6889902259439918E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000F-1CEA-4585-BB20-DDC841D239A5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.1930783955791918E-2"/>
+                  <c:y val="1.6806188912149824E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000E-1CEA-4585-BB20-DDC841D239A5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.5615945782274255E-2"/>
+                  <c:y val="2.0167426694579937E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000D-1CEA-4585-BB20-DDC841D239A5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.2446706611499504E-2"/>
+                  <c:y val="2.6889902259439855E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000B-1CEA-4585-BB20-DDC841D239A5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -300,8 +580,8 @@
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
-                        <a:lumMod val="50000"/>
-                        <a:lumOff val="50000"/>
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -325,13 +605,14 @@
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
-                    <a:ln w="9525">
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                       <a:solidFill>
                         <a:schemeClr val="tx1">
                           <a:lumMod val="35000"/>
                           <a:lumOff val="65000"/>
                         </a:schemeClr>
                       </a:solidFill>
+                      <a:round/>
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
@@ -346,25 +627,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>1.68</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>2.68</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>3.94</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>6.43</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13</c:v>
+                  <c:v>10.15</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21</c:v>
+                  <c:v>14.18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -372,7 +653,294 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-5A49-414F-BAAD-551BD7DC5A21}"/>
+              <c16:uniqueId val="{00000001-1CEA-4585-BB20-DDC841D239A5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Prior</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.7233345897703987E-2"/>
+                  <c:y val="-3.3612377824300023E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-1CEA-4585-BB20-DDC841D239A5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.2761088637427375E-2"/>
+                  <c:y val="-2.3528664477010051E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-1CEA-4585-BB20-DDC841D239A5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.7233345897703969E-2"/>
+                  <c:y val="-3.3612377824299898E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-1CEA-4585-BB20-DDC841D239A5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.2761088637427375E-2"/>
+                  <c:y val="-3.0251140041869906E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-1CEA-4585-BB20-DDC841D239A5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.4603669550668507E-2"/>
+                  <c:y val="-1.6806188912149949E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-1CEA-4585-BB20-DDC841D239A5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.8804754032858296E-2"/>
+                  <c:y val="-1.6806188912149949E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-1CEA-4585-BB20-DDC841D239A5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.6962173119617164E-2"/>
+                  <c:y val="-2.0167426694579969E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-1CEA-4585-BB20-DDC841D239A5}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-1CEA-4585-BB20-DDC841D239A5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -387,30 +955,16 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1784454128"/>
-        <c:axId val="1900263040"/>
+        <c:axId val="2011027136"/>
+        <c:axId val="2068288288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1784454128"/>
+        <c:axId val="2011027136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -420,57 +974,6 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1900263040"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1900263040"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="dk1">
                 <a:lumMod val="15000"/>
                 <a:lumOff val="85000"/>
               </a:schemeClr>
@@ -499,7 +1002,66 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1784454128"/>
+        <c:crossAx val="2068288288"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2068288288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2011027136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -512,7 +1074,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="t"/>
+      <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -548,7 +1110,7 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
@@ -620,7 +1182,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="239">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -631,7 +1193,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" cap="all"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -654,18 +1216,18 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="bg1"/>
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
@@ -677,7 +1239,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -685,11 +1247,11 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -721,45 +1283,35 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="22225" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -771,34 +1323,30 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -820,13 +1368,15 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -841,15 +1391,15 @@
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -860,16 +1410,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -878,10 +1429,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
@@ -897,15 +1448,21 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -924,16 +1481,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="5000"/>
             <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -942,16 +1500,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -960,16 +1519,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -990,7 +1550,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
@@ -998,7 +1558,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -1011,17 +1571,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -1029,10 +1578,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
@@ -1053,7 +1602,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1062,14 +1611,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDash"/>
+        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1083,7 +1632,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="800" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:trendlineLabel>
   <cs:upBar>
     <cs:lnRef idx="0"/>
@@ -1099,8 +1648,8 @@
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1116,17 +1665,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -1134,8 +1672,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -1144,23 +1688,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>43132</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>60385</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>103517</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>34506</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13B381E1-C8FE-412D-8F29-418A24151517}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76FB597C-074D-4C5B-8940-9ADECBFDFC25}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1478,75 +2022,99 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F6E29F2-E4BF-40D5-BD32-70E17339397E}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1.27</v>
       </c>
       <c r="B2">
+        <v>0.1</v>
+      </c>
+      <c r="C2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1.7</v>
       </c>
       <c r="B3">
+        <v>1.68</v>
+      </c>
+      <c r="C3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2.82</v>
       </c>
       <c r="B4">
+        <v>2.68</v>
+      </c>
+      <c r="C4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4.3</v>
       </c>
       <c r="B5">
+        <v>3.94</v>
+      </c>
+      <c r="C5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>7.36</v>
       </c>
       <c r="B6">
+        <v>6.43</v>
+      </c>
+      <c r="C6">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10.210000000000001</v>
       </c>
       <c r="B7">
+        <v>10.15</v>
+      </c>
+      <c r="C7">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>15.72</v>
       </c>
       <c r="B8">
+        <v>14.18</v>
+      </c>
+      <c r="C8">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed machine learning models. finalise 34 data points
</commit_message>
<xml_diff>
--- a/data/GitAndroidAnalysis/accuracy_analysis2/curve_for_weight_adjustment.xlsx
+++ b/data/GitAndroidAnalysis/accuracy_analysis2/curve_for_weight_adjustment.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ResearchSpace\ResearchProjects\UMLx\data\GitAndroidAnalysis\accuracy_analysis2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EB20746-3129-4B9A-B1A8-F4F7C750B79A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA6008B8-AB10-4B20-989D-3D322F1918F7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="21954" windowHeight="11860" xr2:uid="{985EAFBB-D308-49E7-BBB0-9AE92E659F37}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{985EAFBB-D308-49E7-BBB0-9AE92E659F37}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
     <t>Prior</t>
   </si>
@@ -39,6 +40,12 @@
   </si>
   <si>
     <t>SWTII</t>
+  </si>
+  <si>
+    <t>SWTII-AA</t>
+  </si>
+  <si>
+    <t>SWTIII-AA</t>
   </si>
 </sst>
 </file>
@@ -82,6 +89,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFB2B2B2"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -94,6 +106,1394 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Android vs</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Architected Agile (AA)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SWTIII</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-7.3246703865440133E-2"/>
+                  <c:y val="-2.7017890736672503E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>1.16-1.27</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000001F-4BFE-4355-BFFA-2C017FB8E95A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.4491786018901855E-2"/>
+                  <c:y val="1.0807156294668604E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>1.68-1.77</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000001D-4BFE-4355-BFFA-2C017FB8E95A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.1780990453020741E-2"/>
+                  <c:y val="2.1614312589337208E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>2.68-2.99</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000019-4BFE-4355-BFFA-2C017FB8E95A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.0739061603597792E-4"/>
+                  <c:y val="3.2421468884005815E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>3.94-4.45</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000015-4BFE-4355-BFFA-2C017FB8E95A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.3301869126056339E-2"/>
+                  <c:y val="-1.8912523515670056E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000011-4BFE-4355-BFFA-2C017FB8E95A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.27</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.82</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.36</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.210000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15.72</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4BFE-4355-BFFA-2C017FB8E95A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SWTII</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000001C-4BFE-4355-BFFA-2C017FB8E95A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000018-4BFE-4355-BFFA-2C017FB8E95A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000014-4BFE-4355-BFFA-2C017FB8E95A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-9.0701948871398583E-3"/>
+                  <c:y val="1.8912523515670056E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000E-4BFE-4355-BFFA-2C017FB8E95A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$2:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.68</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.68</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.94</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.43</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14.18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4BFE-4355-BFFA-2C017FB8E95A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SWTIII-AA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$D$2:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.1599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.77</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.99</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.45</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.52</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.55</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18.32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4BFE-4355-BFFA-2C017FB8E95A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SWTII-AA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000001E-4BFE-4355-BFFA-2C017FB8E95A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000001A-4BFE-4355-BFFA-2C017FB8E95A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000016-4BFE-4355-BFFA-2C017FB8E95A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000012-4BFE-4355-BFFA-2C017FB8E95A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.9606044860663445E-2"/>
+                  <c:y val="-2.701789073667151E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000010-4BFE-4355-BFFA-2C017FB8E95A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.216711749382706E-2"/>
+                  <c:y val="-2.9719679810338712E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000C-4BFE-4355-BFFA-2C017FB8E95A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$E$2:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.77</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.88</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.42</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.87</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19.190000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-4BFE-4355-BFFA-2C017FB8E95A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Prior</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="bg2">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.6446017206676817E-2"/>
+                  <c:y val="-3.2421468884005912E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000B-4BFE-4355-BFFA-2C017FB8E95A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.1717885405721542E-2"/>
+                  <c:y val="-1.8912523515670156E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-4BFE-4355-BFFA-2C017FB8E95A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.014184147206971E-2"/>
+                  <c:y val="-2.7017890736671511E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-4BFE-4355-BFFA-2C017FB8E95A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.3293929339373264E-2"/>
+                  <c:y val="-2.7017890736671608E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-4BFE-4355-BFFA-2C017FB8E95A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.6446017206676817E-2"/>
+                  <c:y val="-2.4316101663004359E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-4BFE-4355-BFFA-2C017FB8E95A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.1615441309054762E-2"/>
+                  <c:y val="-3.2421468884005863E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-4BFE-4355-BFFA-2C017FB8E95A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.5311265574447538E-2"/>
+                  <c:y val="-3.2421468884005836E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-4BFE-4355-BFFA-2C017FB8E95A}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="bg2">
+                          <a:lumMod val="75000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$2:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-4BFE-4355-BFFA-2C017FB8E95A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1379750128"/>
+        <c:axId val="1134753168"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1379750128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1134753168"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1134753168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1379750128"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -662,7 +2062,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>Sheet1!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -909,7 +2309,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$8</c:f>
+              <c:f>Sheet1!$E$2:$E$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1065,6 +2465,45 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1181,6 +2620,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -1684,17 +3163,561 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>161924</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>185735</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13CD2ED0-DA75-4BB6-A388-6A3DDBA537C2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>43132</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>60385</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>103517</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>34506</xdr:rowOff>
@@ -2021,16 +4044,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F6E29F2-E4BF-40D5-BD32-70E17339397E}">
-  <dimension ref="A1:C8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C3DA7F6-86DF-4BA9-90FE-BBF3D4955AF1}">
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2040,8 +4063,14 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1.27</v>
       </c>
@@ -2051,8 +4080,14 @@
       <c r="C2">
         <v>1</v>
       </c>
+      <c r="D2">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="E2">
+        <v>1.2</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1.7</v>
       </c>
@@ -2062,8 +4097,14 @@
       <c r="C3">
         <v>2</v>
       </c>
+      <c r="D3">
+        <v>1.77</v>
+      </c>
+      <c r="E3">
+        <v>1.77</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2.82</v>
       </c>
@@ -2073,8 +4114,14 @@
       <c r="C4">
         <v>3</v>
       </c>
+      <c r="D4">
+        <v>2.99</v>
+      </c>
+      <c r="E4">
+        <v>2.88</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4.3</v>
       </c>
@@ -2084,8 +4131,14 @@
       <c r="C5">
         <v>5</v>
       </c>
+      <c r="D5">
+        <v>4.45</v>
+      </c>
+      <c r="E5">
+        <v>4.42</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>7.36</v>
       </c>
@@ -2095,8 +4148,14 @@
       <c r="C6">
         <v>8</v>
       </c>
+      <c r="D6">
+        <v>5.52</v>
+      </c>
+      <c r="E6">
+        <v>7.15</v>
+      </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10.210000000000001</v>
       </c>
@@ -2106,8 +4165,14 @@
       <c r="C7">
         <v>13</v>
       </c>
+      <c r="D7">
+        <v>11.55</v>
+      </c>
+      <c r="E7">
+        <v>11.87</v>
+      </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>15.72</v>
       </c>
@@ -2115,6 +4180,164 @@
         <v>14.18</v>
       </c>
       <c r="C8">
+        <v>21</v>
+      </c>
+      <c r="D8">
+        <v>18.32</v>
+      </c>
+      <c r="E8">
+        <v>19.190000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F6E29F2-E4BF-40D5-BD32-70E17339397E}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P26" sqref="P26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1.27</v>
+      </c>
+      <c r="B2">
+        <v>0.1</v>
+      </c>
+      <c r="C2">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="D2">
+        <v>1.2</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1.7</v>
+      </c>
+      <c r="B3">
+        <v>1.68</v>
+      </c>
+      <c r="C3">
+        <v>1.77</v>
+      </c>
+      <c r="D3">
+        <v>1.77</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2.82</v>
+      </c>
+      <c r="B4">
+        <v>2.68</v>
+      </c>
+      <c r="C4">
+        <v>2.99</v>
+      </c>
+      <c r="D4">
+        <v>2.88</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4.3</v>
+      </c>
+      <c r="B5">
+        <v>3.94</v>
+      </c>
+      <c r="C5">
+        <v>4.45</v>
+      </c>
+      <c r="D5">
+        <v>4.42</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>7.36</v>
+      </c>
+      <c r="B6">
+        <v>6.43</v>
+      </c>
+      <c r="C6">
+        <v>5.52</v>
+      </c>
+      <c r="D6">
+        <v>7.15</v>
+      </c>
+      <c r="E6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>10.210000000000001</v>
+      </c>
+      <c r="B7">
+        <v>10.15</v>
+      </c>
+      <c r="C7">
+        <v>11.55</v>
+      </c>
+      <c r="D7">
+        <v>11.87</v>
+      </c>
+      <c r="E7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>15.72</v>
+      </c>
+      <c r="B8">
+        <v>14.18</v>
+      </c>
+      <c r="C8">
+        <v>18.32</v>
+      </c>
+      <c r="D8">
+        <v>13.19</v>
+      </c>
+      <c r="E8">
         <v>21</v>
       </c>
     </row>

</xml_diff>